<commit_message>
Excel importer bug fixed
</commit_message>
<xml_diff>
--- a/modules/ExcelReader/src/main/resources/sample.xlsx
+++ b/modules/ExcelReader/src/main/resources/sample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>Actividad</t>
   </si>
@@ -59,21 +59,6 @@
   </si>
   <si>
     <t>asdas</t>
-  </si>
-  <si>
-    <t>qweqweewq</t>
-  </si>
-  <si>
-    <t>qwewq</t>
-  </si>
-  <si>
-    <t>asddsqweea</t>
-  </si>
-  <si>
-    <t>asdsqweewad</t>
-  </si>
-  <si>
-    <t>dweewasdsa</t>
   </si>
 </sst>
 </file>
@@ -459,7 +444,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -499,8 +484,8 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>15</v>
+      <c r="B3">
+        <v>6575567</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -516,8 +501,8 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
+      <c r="B4">
+        <v>56765</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -533,8 +518,8 @@
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
+      <c r="B5">
+        <v>567765576</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -550,8 +535,8 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
+      <c r="B6">
+        <v>567765</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -567,8 +552,8 @@
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
-        <v>19</v>
+      <c r="B7">
+        <v>567765756</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>

</xml_diff>